<commit_message>
0.1.2: Implement computesRequired flag.
</commit_message>
<xml_diff>
--- a/meta/program/BlancoVeeValidateClassStructure.xlsx
+++ b/meta/program/BlancoVeeValidateClassStructure.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/blanco/blancoVeeValidate/meta/program/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FECA3440-B3A9-0D4F-9F3A-8E093F23CA43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F82287CA-DFEC-D342-9662-30776018AC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18320" yWindow="1480" windowWidth="20080" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23600" yWindow="5980" windowWidth="20080" windowHeight="17440" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="valueObject" sheetId="1" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="82">
   <si>
     <t>バリューオブジェクト定義書</t>
   </si>
@@ -342,16 +342,6 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>認証が必要なクラスかどうか</t>
-    <rPh sb="0" eb="2">
-      <t xml:space="preserve">ニンショウナ </t>
-    </rPh>
-    <rPh sb="3" eb="5">
-      <t xml:space="preserve">ヒツヨウナクラスカドウカ </t>
-    </rPh>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>BlancoVeeValidateClassStructure</t>
     <phoneticPr fontId="3"/>
   </si>
@@ -459,6 +449,39 @@
   </si>
   <si>
     <t>継承するクラスを指定します。</t>
+  </si>
+  <si>
+    <t>computesRequired</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>必須扱いとする。true の時のみ、Schemeクラスに computesRequired: boolean = true; を定義します。</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ニンショウナ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">ヒツヨウナクラスカドウカ </t>
+    </rPh>
+    <rPh sb="14" eb="15">
+      <t xml:space="preserve">トキノミ </t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t>_x0000__x0000__x0002__x0007_</t>
+    </rPh>
+    <rPh sb="64" eb="66">
+      <t/>
+    </rPh>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>メッセージの差し替え</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ニンショウナ </t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t xml:space="preserve">ヒツヨウナクラスカドウカ </t>
+    </rPh>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -993,47 +1016,47 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1445,10 +1468,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G48"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1501,7 +1524,7 @@
       </c>
       <c r="B6" s="6"/>
       <c r="C6" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D6" s="11"/>
       <c r="E6" s="12"/>
@@ -1514,7 +1537,7 @@
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="12"/>
@@ -1527,7 +1550,7 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D8" s="16"/>
       <c r="E8" s="16"/>
@@ -1643,24 +1666,24 @@
       <c r="G18"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="53"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="51"/>
+      <c r="E19" s="54"/>
       <c r="F19"/>
       <c r="G19"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="59"/>
-      <c r="B20" s="60"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="53"/>
+      <c r="A20" s="48"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="51"/>
+      <c r="E20" s="54"/>
       <c r="F20"/>
       <c r="G20"/>
     </row>
@@ -1702,30 +1725,30 @@
       <c r="G24"/>
     </row>
     <row r="25" spans="1:7" ht="13.5" customHeight="1">
-      <c r="A25" s="59" t="s">
+      <c r="A25" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="D25" s="54" t="s">
+      <c r="D25" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="54" t="s">
+      <c r="E25" s="49" t="s">
         <v>6</v>
       </c>
       <c r="F25" s="24"/>
       <c r="G25"/>
     </row>
     <row r="26" spans="1:7">
-      <c r="A26" s="59"/>
-      <c r="B26" s="59"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="54"/>
-      <c r="E26" s="54"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
+      <c r="C26" s="49"/>
+      <c r="D26" s="49"/>
+      <c r="E26" s="49"/>
       <c r="F26" s="9"/>
       <c r="G26"/>
     </row>
@@ -1766,7 +1789,7 @@
     </row>
     <row r="29" spans="1:7" ht="47" customHeight="1">
       <c r="A29" s="38">
-        <f t="shared" ref="A29:A44" si="0">A28+1</f>
+        <f t="shared" ref="A29:A45" si="0">A28+1</f>
         <v>3</v>
       </c>
       <c r="B29" s="39" t="s">
@@ -1776,10 +1799,10 @@
         <v>32</v>
       </c>
       <c r="D29" s="40"/>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="56"/>
+      <c r="F29" s="57"/>
       <c r="G29"/>
     </row>
     <row r="30" spans="1:7" ht="47" customHeight="1">
@@ -1788,16 +1811,16 @@
         <v>4</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="40" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="40"/>
-      <c r="E30" s="55" t="s">
-        <v>63</v>
-      </c>
-      <c r="F30" s="56"/>
+      <c r="E30" s="56" t="s">
+        <v>62</v>
+      </c>
+      <c r="F30" s="57"/>
       <c r="G30"/>
     </row>
     <row r="31" spans="1:7" s="47" customFormat="1" ht="15">
@@ -1806,7 +1829,7 @@
         <v>5</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C31" s="40" t="s">
         <v>41</v>
@@ -1814,10 +1837,10 @@
       <c r="D31" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E31" s="50" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="51"/>
+      <c r="E31" s="52" t="s">
+        <v>72</v>
+      </c>
+      <c r="F31" s="53"/>
       <c r="G31"/>
     </row>
     <row r="32" spans="1:7" s="47" customFormat="1" ht="15">
@@ -1826,7 +1849,7 @@
         <v>6</v>
       </c>
       <c r="B32" s="39" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C32" s="40" t="s">
         <v>41</v>
@@ -1834,10 +1857,10 @@
       <c r="D32" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E32" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="F32" s="58"/>
+      <c r="E32" s="58" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" s="59"/>
       <c r="G32"/>
     </row>
     <row r="33" spans="1:7" ht="47" customHeight="1">
@@ -1852,10 +1875,10 @@
         <v>32</v>
       </c>
       <c r="D33" s="40"/>
-      <c r="E33" s="55" t="s">
+      <c r="E33" s="56" t="s">
         <v>57</v>
       </c>
-      <c r="F33" s="56"/>
+      <c r="F33" s="57"/>
       <c r="G33"/>
     </row>
     <row r="34" spans="1:7" ht="47" customHeight="1">
@@ -1870,10 +1893,10 @@
         <v>32</v>
       </c>
       <c r="D34" s="40"/>
-      <c r="E34" s="55" t="s">
+      <c r="E34" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="F34" s="56"/>
+      <c r="F34" s="57"/>
       <c r="G34"/>
     </row>
     <row r="35" spans="1:7" ht="15">
@@ -1908,10 +1931,10 @@
       <c r="D36" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E36" s="50" t="s">
+      <c r="E36" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="F36" s="51"/>
+      <c r="F36" s="53"/>
       <c r="G36"/>
     </row>
     <row r="37" spans="1:7" ht="15">
@@ -1920,18 +1943,18 @@
         <v>11</v>
       </c>
       <c r="B37" s="39" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C37" s="40" t="s">
         <v>32</v>
       </c>
       <c r="D37" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E37" s="52" t="s">
         <v>76</v>
       </c>
-      <c r="E37" s="50" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="51"/>
+      <c r="F37" s="53"/>
       <c r="G37"/>
     </row>
     <row r="38" spans="1:7" ht="15">
@@ -1940,7 +1963,7 @@
         <v>12</v>
       </c>
       <c r="B38" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C38" s="40" t="s">
         <v>49</v>
@@ -1948,10 +1971,10 @@
       <c r="D38" s="40" t="b">
         <v>0</v>
       </c>
-      <c r="E38" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="F38" s="51"/>
+      <c r="E38" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="53"/>
       <c r="G38"/>
     </row>
     <row r="39" spans="1:7" ht="15">
@@ -1960,18 +1983,18 @@
         <v>13</v>
       </c>
       <c r="B39" s="39" t="s">
-        <v>37</v>
+        <v>79</v>
       </c>
       <c r="C39" s="40" t="s">
         <v>49</v>
       </c>
       <c r="D39" s="40" t="b">
-        <v>1</v>
-      </c>
-      <c r="E39" s="50" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39" s="51"/>
+        <v>0</v>
+      </c>
+      <c r="E39" s="52" t="s">
+        <v>80</v>
+      </c>
+      <c r="F39" s="53"/>
       <c r="G39"/>
     </row>
     <row r="40" spans="1:7" ht="15">
@@ -1980,7 +2003,7 @@
         <v>14</v>
       </c>
       <c r="B40" s="39" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C40" s="40" t="s">
         <v>49</v>
@@ -1988,95 +2011,106 @@
       <c r="D40" s="40" t="b">
         <v>1</v>
       </c>
-      <c r="E40" s="50" t="s">
-        <v>52</v>
-      </c>
-      <c r="F40" s="51"/>
+      <c r="E40" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="53"/>
       <c r="G40"/>
     </row>
-    <row r="41" spans="1:7" s="47" customFormat="1" ht="15">
+    <row r="41" spans="1:7" ht="15">
       <c r="A41" s="38">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B41" s="39" t="s">
-        <v>78</v>
+        <v>51</v>
       </c>
       <c r="C41" s="40" t="s">
-        <v>32</v>
-      </c>
-      <c r="D41" s="40"/>
-      <c r="E41" s="50" t="s">
-        <v>79</v>
-      </c>
-      <c r="F41" s="51"/>
+        <v>49</v>
+      </c>
+      <c r="D41" s="40" t="b">
+        <v>1</v>
+      </c>
+      <c r="E41" s="52" t="s">
+        <v>52</v>
+      </c>
+      <c r="F41" s="53"/>
       <c r="G41"/>
     </row>
-    <row r="42" spans="1:7" ht="45">
+    <row r="42" spans="1:7" s="47" customFormat="1" ht="15">
       <c r="A42" s="38">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B42" s="39" t="s">
-        <v>39</v>
+        <v>77</v>
       </c>
       <c r="C42" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D42" s="40" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="50" t="s">
-        <v>40</v>
-      </c>
-      <c r="F42" s="52"/>
+        <v>32</v>
+      </c>
+      <c r="D42" s="40"/>
+      <c r="E42" s="52" t="s">
+        <v>78</v>
+      </c>
+      <c r="F42" s="53"/>
       <c r="G42"/>
     </row>
-    <row r="43" spans="1:7" ht="15">
+    <row r="43" spans="1:7" ht="45">
       <c r="A43" s="38">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B43" s="39" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="40"/>
-      <c r="E43" s="50" t="s">
-        <v>47</v>
-      </c>
-      <c r="F43" s="52"/>
+        <v>67</v>
+      </c>
+      <c r="D43" s="40" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" s="52" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="55"/>
       <c r="G43"/>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" ht="15">
       <c r="A44" s="38">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B44" s="45" t="s">
+      <c r="B44" s="39" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="40" t="s">
+        <v>48</v>
+      </c>
+      <c r="D44" s="40"/>
+      <c r="E44" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="F44" s="55"/>
+      <c r="G44"/>
+    </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="38">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B45" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="C45" s="46" t="s">
+        <v>70</v>
+      </c>
+      <c r="D45" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E45" s="52" t="s">
         <v>66</v>
       </c>
-      <c r="C44" s="46" t="s">
-        <v>71</v>
-      </c>
-      <c r="D44" s="46" t="s">
-        <v>70</v>
-      </c>
-      <c r="E44" s="50" t="s">
-        <v>67</v>
-      </c>
-      <c r="F44" s="51"/>
-      <c r="G44"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="A45" s="38"/>
-      <c r="B45" s="39"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="40"/>
-      <c r="E45" s="40"/>
-      <c r="F45" s="43"/>
+      <c r="F45" s="53"/>
       <c r="G45"/>
     </row>
     <row r="46" spans="1:7">
@@ -2088,20 +2122,48 @@
       <c r="F46" s="43"/>
       <c r="G46"/>
     </row>
-    <row r="47" spans="1:7" ht="14" customHeight="1">
-      <c r="A47" s="21"/>
-      <c r="B47" s="22"/>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="48"/>
-      <c r="F47" s="49"/>
+    <row r="47" spans="1:7">
+      <c r="A47" s="38"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="43"/>
       <c r="G47"/>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" ht="14" customHeight="1">
+      <c r="A48" s="21"/>
+      <c r="B48" s="22"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="60"/>
+      <c r="F48" s="61"/>
       <c r="G48"/>
     </row>
+    <row r="49" spans="7:7">
+      <c r="G49"/>
+    </row>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="27">
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E40:F40"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E41:F41"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="E25:E26"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E42:F42"/>
     <mergeCell ref="A25:A26"/>
     <mergeCell ref="B25:B26"/>
     <mergeCell ref="C25:C26"/>
@@ -2110,28 +2172,10 @@
     <mergeCell ref="B19:B20"/>
     <mergeCell ref="C19:C20"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="E25:E26"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E41:F41"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E39:F39"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E43:F43"/>
-    <mergeCell ref="E40:F40"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D61" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="D62" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>